<commit_message>
- update DSM exporter - fix unit test - remove typo in documentation
</commit_message>
<xml_diff>
--- a/Development/de.dlr.exchange.excel.trace.xtend/test/data/reference/testReqDSM.xlsx
+++ b/Development/de.dlr.exchange.excel.trace.xtend/test/data/reference/testReqDSM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Design Structure Matrix (DSM)</t>
   </si>
@@ -22,40 +22,28 @@
     <t>testReqTrace</t>
   </si>
   <si>
-    <t>Component 1.1.1| Component 1.1</t>
-  </si>
-  <si>
-    <t>Component 1.2| Component 1</t>
-  </si>
-  <si>
-    <t>Component 2| testReqTrace</t>
-  </si>
-  <si>
-    <t>Component 3| testReqTrace</t>
-  </si>
-  <si>
-    <t>Component 4| testReqTrace</t>
-  </si>
-  <si>
-    <t>Component 6| testReqTrace</t>
-  </si>
-  <si>
-    <t>Component 1.1/ Component 1.1.1</t>
-  </si>
-  <si>
-    <t>Component 1/ Component 1.2</t>
-  </si>
-  <si>
-    <t>testReqTrace/ Component 2</t>
-  </si>
-  <si>
-    <t>testReqTrace/ Component 3</t>
-  </si>
-  <si>
-    <t>testReqTrace/ Component 4</t>
-  </si>
-  <si>
-    <t>testReqTrace/ Component 6</t>
+    <t>Component 1.1.Component 1.1.1</t>
+  </si>
+  <si>
+    <t>Component 1.Component 1.2</t>
+  </si>
+  <si>
+    <t>testReqTrace.Component 2</t>
+  </si>
+  <si>
+    <t>testReqTrace.Component 3</t>
+  </si>
+  <si>
+    <t>testReqTrace.Component 4</t>
+  </si>
+  <si>
+    <t>testReqTrace.Component 6</t>
+  </si>
+  <si>
+    <t>Component 1.1.Component 111</t>
+  </si>
+  <si>
+    <t>Component 1.Component 12</t>
   </si>
 </sst>
 </file>
@@ -114,7 +102,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,18 +115,6 @@
         <bgColor rgb="00FFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF58FA58"/>
-        <bgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -232,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="bottom" horizontal="general"/>
@@ -321,22 +297,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="bottom" horizontal="general" textRotation="90"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general" textRotation="90"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general" textRotation="90"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
       <protection/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -394,7 +354,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="34.87890625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" style="15" customWidth="1"/>
     <col min="3" max="8" width="4.0" style="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -423,16 +383,16 @@
       <c r="H2" s="22"/>
     </row>
     <row r="4">
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="23" t="s">
@@ -469,94 +429,94 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="15">
         <f>COUNTA(C6:H6)</f>
         <v/>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="15">
         <f>COUNTA(C7:H7)</f>
         <v/>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="33"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
     </row>
     <row r="8">
-      <c r="A8" s="26" t="s">
-        <v>10</v>
+      <c r="A8" s="15" t="s">
+        <v>4</v>
       </c>
       <c r="B8" s="15">
         <f>COUNTA(C8:H8)</f>
         <v/>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
     </row>
     <row r="9">
-      <c r="A9" s="27" t="s">
-        <v>11</v>
+      <c r="A9" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="15">
         <f>COUNTA(C9:H9)</f>
         <v/>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B10" s="15">
         <f>COUNTA(C10:H10)</f>
         <v/>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B11" s="15">
         <f>COUNTA(C11:H11)</f>
         <v/>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
     </row>
   </sheetData>
   <sheetProtection/>

</xml_diff>